<commit_message>
refactor(brand): Unificar marca a TestForge en todo el proyecto
- content.ts: brandName, email, copyright → TestForge
- generate-sample.ts: metadata del Excel → TestForge
- Emails: datasetsmx.com → testforge.mx
- Regenerado muestra-gratuita.xlsx con nueva marca

CAMBIOS:
- 8 referencias Datasets MX → TestForge
- Marca 100% consistente en código y assets
- Excel demo actualizado con marca correcta

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/muestras/muestra-gratuita.xlsx
+++ b/public/muestras/muestra-gratuita.xlsx
@@ -997,7 +997,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>MUESTRA GRATUITA - DATASETS MX</v>
+        <v>MUESTRA GRATUITA - TESTFORGE</v>
       </c>
     </row>
     <row r="3">
@@ -1067,7 +1067,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>https://datasetsmx.com</v>
+        <v>https://testforge.mx</v>
       </c>
     </row>
     <row r="17">
@@ -1077,7 +1077,7 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Contacto: hola@datasetsmx.com</v>
+        <v>Contacto: hola@testforge.mx</v>
       </c>
     </row>
   </sheetData>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Datasets MX no se responsabiliza por mal uso.</v>
+        <v>TestForge no se responsabiliza por mal uso.</v>
       </c>
     </row>
     <row r="27">
@@ -1234,7 +1234,7 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>© 2026 Datasets MX. Todos los derechos reservados.</v>
+        <v>© 2026 TestForge. Todos los derechos reservados.</v>
       </c>
     </row>
   </sheetData>

</xml_diff>